<commit_message>
i471--Memory register issue update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/demo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/demo.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\TMP_EIT_suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{E81950D9-FE0A-4DA7-B194-D4998A5010AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,10 +28,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -870,9 +871,6 @@
     <t>suite_path = analysis_00_ta_engine</t>
   </si>
   <si>
-    <t>radiant=ng2_3</t>
-  </si>
-  <si>
     <t>create_clock</t>
   </si>
   <si>
@@ -919,12 +917,15 @@
   </si>
   <si>
     <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --run-par-trce --run-par-iota</t>
+  </si>
+  <si>
+    <t>radiant=ng2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -2009,7 +2010,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2017,13 +2018,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -2083,7 +2084,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2119,22 +2120,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2164,22 +2156,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2194,13 +2180,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2221,64 +2207,31 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2290,7 +2243,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2310,17 +2269,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -2357,19 +2343,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -2405,7 +2391,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4521,7 +4513,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4576,7 +4574,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4621,7 +4625,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4740,7 +4750,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4787,7 +4803,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4823,7 +4845,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F7D95DD5-450F-4A15-90E4-37A80493AD06}" diskRevisions="1" revisionId="644" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DB9EE584-8FC0-4F91-A037-11E2E66D1944}" diskRevisions="1" revisionId="645" version="6">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -4864,6 +4886,14 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{DB9EE584-8FC0-4F91-A037-11E2E66D1944}" dateTime="2023-08-22T21:01:23" maxSheetId="5" userName="Jason Wang" r:id="rId6" minRId="645">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -13445,6 +13475,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="645" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2023</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
@@ -13452,9 +13499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -13492,9 +13539,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13529,7 +13576,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13564,7 +13611,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -13737,10 +13784,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -13796,7 +13845,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -13804,7 +13853,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -13825,23 +13874,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B23" sqref="B23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+      <selection activeCell="C23" sqref="C23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
-      <selection activeCell="C23" sqref="C23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B23" sqref="B23"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -13853,7 +13902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -13894,40 +13943,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
     </row>
     <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -14026,16 +14075,16 @@
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="O3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -14043,16 +14092,16 @@
         <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -14060,16 +14109,16 @@
         <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -14077,16 +14126,16 @@
         <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -14094,16 +14143,16 @@
         <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="O7" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S7" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -14111,83 +14160,83 @@
         <v>79</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S8" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="O9" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AD2"/>
+  <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{A9B67F74-22BB-4DE1-9CF5-640E5E8675C5}"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{09636ED8-99E0-480B-A3C6-CAFDBBF3C337}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:Y2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A2:Y2" xr:uid="{3967EC4B-33C7-4964-AD71-9AC3310B8F76}"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{44D8D95A-CEF1-491F-B179-2EF888C44E6B}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -14196,10 +14245,10 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 G1:H1 C1:E1 A1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 G1:H1 C1:E1 A1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -14208,49 +14257,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$140:$H$140</xm:f>
           </x14:formula1>
           <xm:sqref>AB1:AB1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
           <xm:sqref>AC1:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
@@ -14263,7 +14312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -14328,17 +14377,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="104" t="s">
+      <c r="F111" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="105"/>
-      <c r="H111" s="105"/>
-      <c r="I111" s="105"/>
-      <c r="J111" s="105"/>
-      <c r="K111" s="105"/>
-      <c r="L111" s="105"/>
-      <c r="M111" s="105"/>
-      <c r="N111" s="106"/>
+      <c r="G111" s="69"/>
+      <c r="H111" s="69"/>
+      <c r="I111" s="69"/>
+      <c r="J111" s="69"/>
+      <c r="K111" s="69"/>
+      <c r="L111" s="69"/>
+      <c r="M111" s="69"/>
+      <c r="N111" s="70"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -15202,7 +15251,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="89" t="s">
+      <c r="B147" s="71" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -15228,7 +15277,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="90"/>
+      <c r="B148" s="72"/>
       <c r="C148" s="28" t="s">
         <v>136</v>
       </c>
@@ -15250,7 +15299,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="90"/>
+      <c r="B149" s="72"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -15270,7 +15319,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="90"/>
+      <c r="B150" s="72"/>
       <c r="C150" s="28" t="s">
         <v>138</v>
       </c>
@@ -15294,7 +15343,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="90"/>
+      <c r="B151" s="72"/>
       <c r="C151" s="27" t="s">
         <v>140</v>
       </c>
@@ -15318,7 +15367,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="90"/>
+      <c r="B152" s="72"/>
       <c r="C152" s="27" t="s">
         <v>144</v>
       </c>
@@ -15342,7 +15391,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="90"/>
+      <c r="B153" s="72"/>
       <c r="C153" s="28" t="s">
         <v>147</v>
       </c>
@@ -15364,7 +15413,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="90"/>
+      <c r="B154" s="72"/>
       <c r="C154" s="27" t="s">
         <v>148</v>
       </c>
@@ -15388,7 +15437,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="90"/>
+      <c r="B155" s="72"/>
       <c r="C155" s="27" t="s">
         <v>149</v>
       </c>
@@ -15412,7 +15461,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="90"/>
+      <c r="B156" s="72"/>
       <c r="C156" s="28" t="s">
         <v>150</v>
       </c>
@@ -15436,7 +15485,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="90"/>
+      <c r="B157" s="72"/>
       <c r="C157" s="28" t="s">
         <v>151</v>
       </c>
@@ -15460,7 +15509,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="90"/>
+      <c r="B158" s="72"/>
       <c r="C158" s="28" t="s">
         <v>153</v>
       </c>
@@ -15482,7 +15531,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="84"/>
+      <c r="B159" s="73"/>
       <c r="C159" s="28" t="s">
         <v>56</v>
       </c>
@@ -15506,7 +15555,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="80" t="s">
+      <c r="B160" s="66" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -15532,7 +15581,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="67"/>
       <c r="C161" s="28" t="s">
         <v>161</v>
       </c>
@@ -15556,7 +15605,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="89" t="s">
+      <c r="B162" s="71" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -15580,7 +15629,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="107"/>
+      <c r="B163" s="74"/>
       <c r="C163" s="27" t="s">
         <v>165</v>
       </c>
@@ -15602,7 +15651,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="84"/>
+      <c r="B164" s="73"/>
       <c r="C164" s="27" t="s">
         <v>167</v>
       </c>
@@ -15622,7 +15671,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="80" t="s">
+      <c r="B165" s="66" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -15646,7 +15695,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="79"/>
+      <c r="B166" s="67"/>
       <c r="C166" s="28" t="s">
         <v>172</v>
       </c>
@@ -15666,7 +15715,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="67"/>
       <c r="C167" s="28" t="s">
         <v>173</v>
       </c>
@@ -15686,7 +15735,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="67"/>
       <c r="C168" s="28" t="s">
         <v>174</v>
       </c>
@@ -15706,7 +15755,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="79"/>
+      <c r="B169" s="67"/>
       <c r="C169" s="28" t="s">
         <v>175</v>
       </c>
@@ -15726,7 +15775,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="67"/>
       <c r="C170" s="28" t="s">
         <v>176</v>
       </c>
@@ -15746,7 +15795,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="67"/>
       <c r="C171" s="28" t="s">
         <v>177</v>
       </c>
@@ -15766,7 +15815,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="79"/>
+      <c r="B172" s="67"/>
       <c r="C172" s="28" t="s">
         <v>41</v>
       </c>
@@ -15786,7 +15835,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="80" t="s">
+      <c r="B173" s="66" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -15810,7 +15859,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="79"/>
+      <c r="B174" s="67"/>
       <c r="C174" s="27" t="s">
         <v>181</v>
       </c>
@@ -15832,7 +15881,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="79"/>
+      <c r="B175" s="67"/>
       <c r="C175" s="28" t="s">
         <v>184</v>
       </c>
@@ -15854,7 +15903,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="89" t="s">
+      <c r="B176" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -15880,7 +15929,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="90"/>
+      <c r="B177" s="72"/>
       <c r="C177" s="32" t="s">
         <v>189</v>
       </c>
@@ -15904,7 +15953,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="91" t="s">
+      <c r="B178" s="75" t="s">
         <v>191</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -15928,7 +15977,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="92"/>
+      <c r="B179" s="76"/>
       <c r="C179" s="27" t="s">
         <v>195</v>
       </c>
@@ -15950,7 +15999,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="93"/>
+      <c r="B180" s="77"/>
       <c r="C180" s="34" t="s">
         <v>198</v>
       </c>
@@ -15972,7 +16021,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="93"/>
+      <c r="B181" s="77"/>
       <c r="C181" s="34" t="s">
         <v>199</v>
       </c>
@@ -15994,17 +16043,17 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="93"/>
+      <c r="B182" s="77"/>
       <c r="C182" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F182" s="42"/>
+      <c r="F182" s="32"/>
       <c r="G182" s="34" t="s">
         <v>260</v>
       </c>
@@ -16014,15 +16063,15 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="93"/>
+      <c r="B183" s="77"/>
       <c r="C183" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E183" s="42"/>
-      <c r="F183" s="42" t="s">
+      <c r="E183" s="32"/>
+      <c r="F183" s="32" t="s">
         <v>255</v>
       </c>
       <c r="G183" s="34" t="s">
@@ -16036,7 +16085,7 @@
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="88"/>
+      <c r="B184" s="78"/>
       <c r="C184" s="36" t="s">
         <v>258</v>
       </c>
@@ -16063,7 +16112,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="6" t="s">
         <v>205</v>
       </c>
     </row>
@@ -16084,280 +16133,280 @@
       <c r="A198" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B198" s="38" t="s">
+      <c r="B198" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C198" s="94" t="s">
+      <c r="C198" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D198" s="94"/>
-      <c r="E198" s="94"/>
-      <c r="F198" s="39" t="s">
+      <c r="D198" s="79"/>
+      <c r="E198" s="79"/>
+      <c r="F198" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="G198" s="40" t="s">
+      <c r="G198" s="38" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="77" t="s">
+      <c r="A199" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="79" t="s">
+      <c r="B199" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D199" s="97"/>
-      <c r="E199" s="97"/>
+      <c r="D199" s="83"/>
+      <c r="E199" s="83"/>
       <c r="F199" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G199" s="41" t="s">
+      <c r="G199" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="77"/>
-      <c r="B200" s="95"/>
-      <c r="C200" s="98" t="s">
+      <c r="A200" s="80"/>
+      <c r="B200" s="81"/>
+      <c r="C200" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="85"/>
+      <c r="E200" s="85"/>
       <c r="F200" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="G200" s="43" t="s">
+      <c r="G200" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="77"/>
-      <c r="B201" s="79" t="s">
+      <c r="A201" s="80"/>
+      <c r="B201" s="67" t="s">
         <v>216</v>
       </c>
-      <c r="C201" s="100" t="s">
+      <c r="C201" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="D201" s="100"/>
-      <c r="E201" s="100"/>
+      <c r="D201" s="86"/>
+      <c r="E201" s="86"/>
       <c r="F201" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G201" s="41" t="s">
+      <c r="G201" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="77"/>
-      <c r="B202" s="79"/>
-      <c r="C202" s="98" t="s">
+      <c r="A202" s="80"/>
+      <c r="B202" s="67"/>
+      <c r="C202" s="84" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="98"/>
-      <c r="E202" s="98"/>
+      <c r="D202" s="84"/>
+      <c r="E202" s="84"/>
       <c r="F202" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="77"/>
-      <c r="B203" s="95" t="s">
+      <c r="A203" s="80"/>
+      <c r="B203" s="81" t="s">
         <v>218</v>
       </c>
-      <c r="C203" s="101" t="s">
+      <c r="C203" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D203" s="102"/>
-      <c r="E203" s="103"/>
+      <c r="D203" s="88"/>
+      <c r="E203" s="89"/>
       <c r="F203" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="77"/>
-      <c r="B204" s="84"/>
-      <c r="C204" s="101" t="s">
+      <c r="A204" s="80"/>
+      <c r="B204" s="73"/>
+      <c r="C204" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="102"/>
-      <c r="E204" s="103"/>
+      <c r="D204" s="88"/>
+      <c r="E204" s="89"/>
       <c r="F204" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="77"/>
-      <c r="B205" s="79" t="s">
+      <c r="A205" s="80"/>
+      <c r="B205" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="C205" s="100" t="s">
+      <c r="C205" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="D205" s="100"/>
-      <c r="E205" s="100"/>
+      <c r="D205" s="86"/>
+      <c r="E205" s="86"/>
       <c r="F205" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="77"/>
-      <c r="B206" s="79"/>
-      <c r="C206" s="100" t="s">
+      <c r="A206" s="80"/>
+      <c r="B206" s="67"/>
+      <c r="C206" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="100"/>
-      <c r="E206" s="100"/>
+      <c r="D206" s="86"/>
+      <c r="E206" s="86"/>
       <c r="F206" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="77" t="s">
+      <c r="A207" s="80" t="s">
         <v>221</v>
       </c>
-      <c r="B207" s="79" t="s">
+      <c r="B207" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="C207" s="80" t="s">
+      <c r="C207" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D207" s="79"/>
-      <c r="E207" s="79"/>
+      <c r="D207" s="67"/>
+      <c r="E207" s="67"/>
       <c r="F207" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="77"/>
-      <c r="B208" s="79"/>
-      <c r="C208" s="79" t="s">
+      <c r="A208" s="80"/>
+      <c r="B208" s="67"/>
+      <c r="C208" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="D208" s="79"/>
-      <c r="E208" s="79"/>
+      <c r="D208" s="67"/>
+      <c r="E208" s="67"/>
       <c r="F208" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="77"/>
-      <c r="B209" s="79" t="s">
+      <c r="A209" s="80"/>
+      <c r="B209" s="67" t="s">
         <v>224</v>
       </c>
-      <c r="C209" s="79" t="s">
+      <c r="C209" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D209" s="79"/>
-      <c r="E209" s="79"/>
+      <c r="D209" s="67"/>
+      <c r="E209" s="67"/>
       <c r="F209" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="77"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="79" t="s">
+      <c r="A210" s="80"/>
+      <c r="B210" s="67"/>
+      <c r="C210" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="D210" s="79"/>
-      <c r="E210" s="79"/>
+      <c r="D210" s="67"/>
+      <c r="E210" s="67"/>
       <c r="F210" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="77" t="s">
+      <c r="A211" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="B211" s="79" t="s">
+      <c r="B211" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="C211" s="80" t="s">
+      <c r="C211" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D211" s="79"/>
-      <c r="E211" s="79"/>
+      <c r="D211" s="67"/>
+      <c r="E211" s="67"/>
       <c r="F211" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="77"/>
-      <c r="B212" s="79"/>
-      <c r="C212" s="79" t="s">
+      <c r="A212" s="80"/>
+      <c r="B212" s="67"/>
+      <c r="C212" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="79"/>
-      <c r="E212" s="79"/>
+      <c r="D212" s="67"/>
+      <c r="E212" s="67"/>
       <c r="F212" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="77"/>
-      <c r="B213" s="79" t="s">
+      <c r="A213" s="80"/>
+      <c r="B213" s="67" t="s">
         <v>227</v>
       </c>
-      <c r="C213" s="80" t="s">
+      <c r="C213" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="D213" s="79"/>
-      <c r="E213" s="79"/>
+      <c r="D213" s="67"/>
+      <c r="E213" s="67"/>
       <c r="F213" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="78"/>
-      <c r="B214" s="81"/>
-      <c r="C214" s="81" t="s">
+      <c r="A214" s="91"/>
+      <c r="B214" s="92"/>
+      <c r="C214" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="92"/>
+      <c r="E214" s="92"/>
       <c r="F214" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="G214" s="44" t="s">
+      <c r="G214" s="41" t="s">
         <v>63</v>
       </c>
     </row>
@@ -16365,60 +16414,43 @@
       <c r="A215" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C215" s="37"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="37"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
     </row>
     <row r="218" spans="1:7" ht="15.75" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
     </row>
     <row r="219" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A219" s="45" t="s">
+      <c r="A219" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="B219" s="82" t="s">
+      <c r="B219" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="C219" s="82"/>
-      <c r="D219" s="82"/>
-      <c r="E219" s="82"/>
-      <c r="F219" s="46" t="s">
+      <c r="C219" s="93"/>
+      <c r="D219" s="93"/>
+      <c r="E219" s="93"/>
+      <c r="F219" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G219" s="47" t="s">
+      <c r="G219" s="44" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="93" customHeight="1">
-      <c r="A220" s="48" t="s">
+      <c r="A220" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="B220" s="83" t="s">
+      <c r="B220" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
-      <c r="F220" s="49" t="s">
+      <c r="C220" s="73"/>
+      <c r="D220" s="73"/>
+      <c r="E220" s="73"/>
+      <c r="F220" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="G220" s="50" t="s">
+      <c r="G220" s="47" t="s">
         <v>63</v>
       </c>
     </row>
@@ -16426,12 +16458,12 @@
       <c r="A221" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="87"/>
+      <c r="C221" s="96"/>
+      <c r="D221" s="96"/>
+      <c r="E221" s="97"/>
       <c r="F221" s="15" t="s">
         <v>63</v>
       </c>
@@ -16443,12 +16475,12 @@
       <c r="A222" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B222" s="85" t="s">
+      <c r="B222" s="95" t="s">
         <v>239</v>
       </c>
-      <c r="C222" s="86"/>
-      <c r="D222" s="86"/>
-      <c r="E222" s="87"/>
+      <c r="C222" s="96"/>
+      <c r="D222" s="96"/>
+      <c r="E222" s="97"/>
       <c r="F222" s="18" t="s">
         <v>63</v>
       </c>
@@ -16460,12 +16492,12 @@
       <c r="A223" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B223" s="88" t="s">
+      <c r="B223" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="C223" s="81"/>
-      <c r="D223" s="81"/>
-      <c r="E223" s="81"/>
+      <c r="C223" s="92"/>
+      <c r="D223" s="92"/>
+      <c r="E223" s="92"/>
       <c r="F223" s="21" t="s">
         <v>63</v>
       </c>
@@ -16474,7 +16506,7 @@
       </c>
     </row>
     <row r="224" spans="1:7">
-      <c r="C224" s="51"/>
+      <c r="C224" s="48"/>
     </row>
     <row r="226" spans="1:7" ht="15.75" thickBot="1">
       <c r="A226" s="6" t="s">
@@ -16485,280 +16517,303 @@
       <c r="A227" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B227" s="38" t="s">
+      <c r="B227" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C227" s="52" t="s">
+      <c r="C227" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D227" s="53" t="s">
+      <c r="D227" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E227" s="53"/>
-      <c r="F227" s="54"/>
-      <c r="G227" s="40" t="s">
+      <c r="E227" s="50"/>
+      <c r="F227" s="10"/>
+      <c r="G227" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="55">
+      <c r="A228" s="51">
         <v>42682</v>
       </c>
-      <c r="B228" s="56">
+      <c r="B228" s="52">
         <v>1.04</v>
       </c>
       <c r="C228" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D228" s="76" t="s">
+      <c r="D228" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="E228" s="76"/>
-      <c r="F228" s="76"/>
-      <c r="G228" s="57"/>
+      <c r="E228" s="90"/>
+      <c r="F228" s="90"/>
+      <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="58">
+      <c r="A229" s="53">
         <v>42692</v>
       </c>
-      <c r="B229" s="59">
+      <c r="B229" s="54">
         <v>1.05</v>
       </c>
       <c r="C229" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="75" t="s">
+      <c r="D229" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="E229" s="75"/>
-      <c r="F229" s="75"/>
-      <c r="G229" s="41"/>
+      <c r="E229" s="102"/>
+      <c r="F229" s="102"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42955</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.06</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="75" t="s">
+      <c r="D230" s="102" t="s">
         <v>245</v>
       </c>
-      <c r="E230" s="75"/>
-      <c r="F230" s="75"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="102"/>
+      <c r="F230" s="102"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42991</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.07</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="75" t="s">
+      <c r="D231" s="102" t="s">
         <v>246</v>
       </c>
-      <c r="E231" s="75"/>
-      <c r="F231" s="75"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="102"/>
+      <c r="F231" s="102"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>43026</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.08</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="75" t="s">
+      <c r="D232" s="102" t="s">
         <v>247</v>
       </c>
-      <c r="E232" s="75"/>
-      <c r="F232" s="75"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="102"/>
+      <c r="F232" s="102"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43069</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="75" t="s">
+      <c r="D233" s="102" t="s">
         <v>248</v>
       </c>
-      <c r="E233" s="75"/>
-      <c r="F233" s="75"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="102"/>
+      <c r="F233" s="102"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="60">
+      <c r="A234" s="55">
         <v>43248</v>
       </c>
-      <c r="B234" s="61">
+      <c r="B234" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="71" t="s">
+      <c r="D234" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="E234" s="72"/>
-      <c r="F234" s="73"/>
-      <c r="G234" s="43"/>
+      <c r="E234" s="99"/>
+      <c r="F234" s="100"/>
+      <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43339</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="71" t="s">
+      <c r="D235" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="E235" s="72"/>
-      <c r="F235" s="73"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="99"/>
+      <c r="F235" s="100"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43542</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="71" t="s">
+      <c r="D236" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="E236" s="72"/>
-      <c r="F236" s="73"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="99"/>
+      <c r="F236" s="100"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43599</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="62" t="s">
+      <c r="D237" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="E237" s="63"/>
-      <c r="F237" s="64"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="58"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43643</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43894</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>44017</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A241" s="65">
+      <c r="A241" s="60">
         <v>44118</v>
       </c>
-      <c r="B241" s="66">
+      <c r="B241" s="61">
         <v>1.17</v>
       </c>
       <c r="C241" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D241" s="74" t="s">
+      <c r="D241" s="101" t="s">
         <v>261</v>
       </c>
-      <c r="E241" s="74"/>
-      <c r="F241" s="74"/>
-      <c r="G241" s="44"/>
+      <c r="E241" s="101"/>
+      <c r="F241" s="101"/>
+      <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -16775,35 +16830,12 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -16812,7 +16844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16826,18 +16858,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i512--Password hide, eit2 demo update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/demo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/demo.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92583CAC-3003-4933-ADE0-A8C57DFC9584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B260FDE2-109E-44C5-B74B-E4F9AA24DC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bAnXdR/C/TexoDwtCiyJUp1QPcnLokb+nXtWHUMutRp3/JwbfmvQ9OTszxPHu099kEsZRnm77cQtrH/+R8sQQQ==" workbookSaltValue="jEKgPqypKRsX/tR/dxCvHg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="350">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -725,9 +725,6 @@
   </si>
   <si>
     <t>Author column added</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
   <si>
     <t>OS property update</t>
@@ -1047,27 +1044,15 @@
     <t>override support for Caseinfo, Software, System, Machine and Preference</t>
   </si>
   <si>
-    <t>Robinson Meng</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>analysis_00_ta_engine</t>
-  </si>
-  <si>
     <t>repository = http://lsh-tmp/radiant/trunk/general</t>
   </si>
   <si>
     <t>suite_path = analysis_00_ta_engine</t>
   </si>
   <si>
-    <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --run-par-trce --run-par-iota</t>
-  </si>
-  <si>
-    <t>radiant=ng2023</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -1083,46 +1068,55 @@
     <t>6</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>create_clock</t>
-  </si>
-  <si>
-    <t>SDC_cases/01_create_clock/get_nets_01</t>
-  </si>
-  <si>
-    <t>SDC_cases/01_create_clock/get_pins_02</t>
-  </si>
-  <si>
-    <t>SDC_cases/01_create_clock/get_ports_01</t>
-  </si>
-  <si>
-    <t>SDC_cases/01_create_clock/two_clocks_nets_ports_01</t>
-  </si>
-  <si>
-    <t>create_generated_clock</t>
-  </si>
-  <si>
-    <t>SDC_cases/02_create_generated_clock/divideby_cells_01</t>
-  </si>
-  <si>
-    <t>SDC_cases/02_create_generated_clock/divideby_nets_01</t>
-  </si>
-  <si>
-    <t>SDC_cases/02_create_generated_clock/divideby_pins_01</t>
-  </si>
-  <si>
-    <t>set_clock_uncertainty</t>
-  </si>
-  <si>
-    <t>SDC_cases/04_set_clock_uncertainty/fallfrom_riseto_01</t>
-  </si>
-  <si>
-    <t>cmd = --devkit=iCE40UP5K-CM225I</t>
-  </si>
-  <si>
-    <t>Command</t>
+    <t>01_timing_constraint</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/101_get_nets_waveform</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_net, option use -waveform</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/102_get_pins_waveform</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_pin, option use -waveform</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/103_get_ports_no_waveform</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_port, option no use -waveform</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/104_get_ports_waveform</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_port, option use -waveform(decimal)</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/105_get_ports_waveform</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_port, option use -waveform(not from 0)</t>
+  </si>
+  <si>
+    <t>01_timing_constraint/01_create_clock/106_get_ports_waveform_negedge</t>
+  </si>
+  <si>
+    <t>create_clock: object use get_port, option use -waveform and negedge clk</t>
+  </si>
+  <si>
+    <t>radiant=ng2024</t>
+  </si>
+  <si>
+    <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse  --run-par-trce</t>
+  </si>
+  <si>
+    <t>eit2_regression_demo</t>
+  </si>
+  <si>
+    <t>Jason.Wang</t>
   </si>
 </sst>
 </file>
@@ -1917,20 +1911,50 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1938,12 +1962,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1956,16 +1974,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
@@ -1985,32 +1997,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -5047,8 +5041,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5063,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5071,7 +5065,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5079,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5087,12 +5081,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="47" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5105,7 +5099,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5113,7 +5107,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5134,8 +5128,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5144,8 +5138,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5158,13 +5152,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5273,7 +5267,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N2" s="49" t="s">
         <v>3</v>
@@ -5338,161 +5332,109 @@
         <v>36</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>340</v>
-      </c>
-      <c r="P3" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T3" s="47" t="s">
-        <v>351</v>
+        <v>334</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>333</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>339</v>
-      </c>
       <c r="E4" s="47" t="s">
-        <v>341</v>
-      </c>
-      <c r="P4" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T4" s="47" t="s">
-        <v>351</v>
+        <v>336</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="47" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D5" s="47" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="H5" s="47" t="s">
         <v>339</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>342</v>
-      </c>
-      <c r="P5" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T5" s="47" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="47" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>343</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T6" s="47" t="s">
-        <v>351</v>
+        <v>340</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:32">
       <c r="A7" s="47" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>345</v>
-      </c>
-      <c r="P7" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T7" s="47" t="s">
-        <v>351</v>
+        <v>342</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="47" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D8" s="47" t="s">
+        <v>333</v>
+      </c>
+      <c r="E8" s="47" t="s">
         <v>344</v>
       </c>
-      <c r="E8" s="47" t="s">
-        <v>346</v>
-      </c>
-      <c r="P8" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T8" s="47" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
-      <c r="A9" s="47" t="s">
-        <v>338</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>344</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>347</v>
-      </c>
-      <c r="P9" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T9" s="47" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32">
-      <c r="A10" s="47" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>348</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>349</v>
-      </c>
-      <c r="P10" s="47" t="s">
-        <v>350</v>
-      </c>
-      <c r="T10" s="47" t="s">
-        <v>351</v>
+      <c r="H8" s="47" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="87B7huxoL3M671d/HVLeYwUvn1T5Ug7j2M+kqBiozhPdXA8hQ5kzEi3j/oT74dCmtfEjRH4zRkkJ7gyPNnbl1w==" saltValue="aF7n9kFinT3G7LRR7PxlDg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AF2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46" xr:uid="{45CDFB6D-4AAF-4DCA-9533-22B828B2316B}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{27021081-22EF-4698-A4F1-E4BDA4C9CF30}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{1831BFF2-1D5F-42D8-9434-922FC2EBC75A}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{256D95B6-4570-44D7-8C65-077344CBF1F1}"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{62173C11-3B81-41CE-AE57-0FC5A9C6FF5B}"/>
+      <autoFilter ref="A2:AF46" xr:uid="{B7B46EC4-7A38-4220-88A9-7337484F0910}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -5576,7 +5518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EE01F-5779-44D2-888C-0F22BF031381}">
   <dimension ref="A1:N290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C216" sqref="C216:H216"/>
     </sheetView>
   </sheetViews>
@@ -5638,17 +5580,17 @@
       <c r="E111" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F111" s="82" t="s">
+      <c r="F111" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="G111" s="83"/>
-      <c r="H111" s="83"/>
-      <c r="I111" s="83"/>
-      <c r="J111" s="83"/>
-      <c r="K111" s="83"/>
-      <c r="L111" s="83"/>
-      <c r="M111" s="83"/>
-      <c r="N111" s="84"/>
+      <c r="G111" s="113"/>
+      <c r="H111" s="113"/>
+      <c r="I111" s="113"/>
+      <c r="J111" s="113"/>
+      <c r="K111" s="113"/>
+      <c r="L111" s="113"/>
+      <c r="M111" s="113"/>
+      <c r="N111" s="114"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -5990,7 +5932,7 @@
     </row>
     <row r="124" spans="1:14">
       <c r="A124" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>52</v>
@@ -6568,7 +6510,7 @@
       <c r="A149" s="63">
         <v>1</v>
       </c>
-      <c r="B149" s="85" t="s">
+      <c r="B149" s="95" t="s">
         <v>3</v>
       </c>
       <c r="C149" s="64" t="s">
@@ -6594,7 +6536,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="86"/>
+      <c r="B150" s="96"/>
       <c r="C150" s="21" t="s">
         <v>82</v>
       </c>
@@ -6616,7 +6558,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="86"/>
+      <c r="B151" s="96"/>
       <c r="C151" s="21" t="s">
         <v>16</v>
       </c>
@@ -6636,7 +6578,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="86"/>
+      <c r="B152" s="96"/>
       <c r="C152" s="21" t="s">
         <v>84</v>
       </c>
@@ -6660,7 +6602,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="86"/>
+      <c r="B153" s="96"/>
       <c r="C153" s="51" t="s">
         <v>86</v>
       </c>
@@ -6684,7 +6626,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="86"/>
+      <c r="B154" s="96"/>
       <c r="C154" s="51" t="s">
         <v>90</v>
       </c>
@@ -6708,7 +6650,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="86"/>
+      <c r="B155" s="96"/>
       <c r="C155" s="21" t="s">
         <v>92</v>
       </c>
@@ -6730,7 +6672,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="86"/>
+      <c r="B156" s="96"/>
       <c r="C156" s="51" t="s">
         <v>93</v>
       </c>
@@ -6754,7 +6696,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="86"/>
+      <c r="B157" s="96"/>
       <c r="C157" s="51" t="s">
         <v>94</v>
       </c>
@@ -6778,7 +6720,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="86"/>
+      <c r="B158" s="96"/>
       <c r="C158" s="21" t="s">
         <v>95</v>
       </c>
@@ -6802,7 +6744,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="86"/>
+      <c r="B159" s="96"/>
       <c r="C159" s="21" t="s">
         <v>96</v>
       </c>
@@ -6826,7 +6768,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="86"/>
+      <c r="B160" s="96"/>
       <c r="C160" s="21" t="s">
         <v>98</v>
       </c>
@@ -6848,51 +6790,51 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="86"/>
+      <c r="B161" s="96"/>
       <c r="C161" s="51" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D161" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E161" s="21"/>
       <c r="F161" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="G161" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="H161" s="54" t="s">
         <v>319</v>
-      </c>
-      <c r="G161" s="51" t="s">
-        <v>318</v>
-      </c>
-      <c r="H161" s="54" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="86"/>
+      <c r="B162" s="96"/>
       <c r="C162" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E162" s="21"/>
       <c r="F162" s="51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G162" s="51" t="s">
+        <v>313</v>
+      </c>
+      <c r="H162" s="54" t="s">
         <v>314</v>
-      </c>
-      <c r="H162" s="54" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="86"/>
+      <c r="B163" s="96"/>
       <c r="C163" s="51" t="s">
         <v>102</v>
       </c>
@@ -6916,7 +6858,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="87"/>
+      <c r="B164" s="89"/>
       <c r="C164" s="21" t="s">
         <v>113</v>
       </c>
@@ -6927,20 +6869,20 @@
         <v>78</v>
       </c>
       <c r="F164" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G164" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="H164" s="11" t="s">
         <v>322</v>
-      </c>
-      <c r="H164" s="11" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="80" t="s">
+      <c r="B165" s="85" t="s">
         <v>4</v>
       </c>
       <c r="C165" s="21" t="s">
@@ -6967,33 +6909,33 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="80"/>
+      <c r="B166" s="85"/>
       <c r="C166" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="D166" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E166" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F166" s="55" t="s">
         <v>244</v>
-      </c>
-      <c r="D166" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E166" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F166" s="55" t="s">
-        <v>245</v>
       </c>
       <c r="G166" s="51" t="s">
         <v>80</v>
       </c>
       <c r="H166" s="54" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="80"/>
+      <c r="B167" s="85"/>
       <c r="C167" s="51" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D167" s="21" t="s">
         <v>78</v>
@@ -7002,22 +6944,22 @@
         <v>78</v>
       </c>
       <c r="F167" s="55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G167" s="51" t="s">
         <v>80</v>
       </c>
       <c r="H167" s="54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="80"/>
+      <c r="B168" s="85"/>
       <c r="C168" s="70" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D168" s="21" t="s">
         <v>78</v>
@@ -7029,19 +6971,19 @@
         <v>0</v>
       </c>
       <c r="G168" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="H168" s="71" t="s">
         <v>282</v>
-      </c>
-      <c r="H168" s="71" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="80"/>
+      <c r="B169" s="85"/>
       <c r="C169" s="70" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D169" s="21" t="s">
         <v>78</v>
@@ -7053,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="G169" s="70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H169" s="71"/>
     </row>
@@ -7061,9 +7003,9 @@
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="80"/>
+      <c r="B170" s="85"/>
       <c r="C170" s="70" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D170" s="21" t="s">
         <v>78</v>
@@ -7075,7 +7017,7 @@
         <v>1</v>
       </c>
       <c r="G170" s="70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H170" s="54"/>
     </row>
@@ -7083,9 +7025,9 @@
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="80"/>
+      <c r="B171" s="85"/>
       <c r="C171" s="70" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D171" s="21" t="s">
         <v>78</v>
@@ -7097,17 +7039,17 @@
         <v>1</v>
       </c>
       <c r="G171" s="70" t="s">
+        <v>308</v>
+      </c>
+      <c r="H171" s="54" t="s">
         <v>309</v>
-      </c>
-      <c r="H171" s="54" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="80"/>
+      <c r="B172" s="85"/>
       <c r="C172" s="70" t="s">
         <v>109</v>
       </c>
@@ -7129,7 +7071,7 @@
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="81"/>
+      <c r="B173" s="84"/>
       <c r="C173" s="51" t="s">
         <v>113</v>
       </c>
@@ -7140,13 +7082,13 @@
         <v>78</v>
       </c>
       <c r="F173" s="55" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G173" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="H173" s="71" t="s">
         <v>322</v>
-      </c>
-      <c r="H173" s="71" t="s">
-        <v>323</v>
       </c>
       <c r="I173" s="59"/>
     </row>
@@ -7154,7 +7096,7 @@
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="88" t="s">
+      <c r="B174" s="94" t="s">
         <v>5</v>
       </c>
       <c r="C174" s="51" t="s">
@@ -7173,7 +7115,7 @@
         <v>80</v>
       </c>
       <c r="H174" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I174" s="59"/>
     </row>
@@ -7181,9 +7123,9 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="85"/>
+      <c r="B175" s="95"/>
       <c r="C175" s="70" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D175" s="21" t="s">
         <v>78</v>
@@ -7192,22 +7134,22 @@
         <v>78</v>
       </c>
       <c r="F175" s="51" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G175" s="51" t="s">
         <v>80</v>
       </c>
       <c r="H175" s="54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="85"/>
+      <c r="B176" s="95"/>
       <c r="C176" s="70" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D176" s="21" t="s">
         <v>78</v>
@@ -7216,22 +7158,22 @@
         <v>78</v>
       </c>
       <c r="F176" s="51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G176" s="51" t="s">
         <v>80</v>
       </c>
       <c r="H176" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="85"/>
+      <c r="B177" s="95"/>
       <c r="C177" s="70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D177" s="21" t="s">
         <v>78</v>
@@ -7240,7 +7182,7 @@
         <v>78</v>
       </c>
       <c r="F177" s="51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G177" s="51" t="s">
         <v>80</v>
@@ -7251,9 +7193,9 @@
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="85"/>
+      <c r="B178" s="95"/>
       <c r="C178" s="70" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D178" s="21" t="s">
         <v>78</v>
@@ -7262,7 +7204,7 @@
         <v>78</v>
       </c>
       <c r="F178" s="51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G178" s="51" t="s">
         <v>80</v>
@@ -7273,31 +7215,31 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="85"/>
+      <c r="B179" s="95"/>
       <c r="C179" s="51" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D179" s="21"/>
       <c r="E179" s="21" t="s">
         <v>78</v>
       </c>
       <c r="F179" s="51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G179" s="51" t="s">
         <v>80</v>
       </c>
       <c r="H179" s="60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="85"/>
+      <c r="B180" s="95"/>
       <c r="C180" s="70" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D180" s="21" t="s">
         <v>78</v>
@@ -7306,22 +7248,22 @@
         <v>78</v>
       </c>
       <c r="F180" s="70" t="s">
+        <v>275</v>
+      </c>
+      <c r="G180" s="70" t="s">
+        <v>287</v>
+      </c>
+      <c r="H180" s="60" t="s">
         <v>276</v>
-      </c>
-      <c r="G180" s="70" t="s">
-        <v>288</v>
-      </c>
-      <c r="H180" s="60" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="181" spans="1:8">
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="85"/>
+      <c r="B181" s="95"/>
       <c r="C181" s="51" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D181" s="70" t="s">
         <v>78</v>
@@ -7334,16 +7276,16 @@
         <v>137</v>
       </c>
       <c r="H181" s="54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="182" spans="1:8">
       <c r="A182" s="19">
         <v>34</v>
       </c>
-      <c r="B182" s="85"/>
+      <c r="B182" s="95"/>
       <c r="C182" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D182" s="70" t="s">
         <v>78</v>
@@ -7352,20 +7294,20 @@
         <v>78</v>
       </c>
       <c r="F182" s="70" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G182" s="70" t="s">
+        <v>284</v>
+      </c>
+      <c r="H182" s="71" t="s">
         <v>285</v>
-      </c>
-      <c r="H182" s="71" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" s="19">
         <v>35</v>
       </c>
-      <c r="B183" s="85"/>
+      <c r="B183" s="95"/>
       <c r="C183" s="51" t="s">
         <v>211</v>
       </c>
@@ -7380,14 +7322,14 @@
         <v>80</v>
       </c>
       <c r="H183" s="54" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="A184" s="19">
         <v>36</v>
       </c>
-      <c r="B184" s="87"/>
+      <c r="B184" s="89"/>
       <c r="C184" s="51" t="s">
         <v>113</v>
       </c>
@@ -7401,17 +7343,17 @@
         <v>226</v>
       </c>
       <c r="G184" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H184" s="60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="185" spans="1:8">
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="80" t="s">
+      <c r="B185" s="85" t="s">
         <v>6</v>
       </c>
       <c r="C185" s="21" t="s">
@@ -7427,41 +7369,41 @@
         <v>115</v>
       </c>
       <c r="G185" s="51" t="s">
+        <v>260</v>
+      </c>
+      <c r="H185" s="54" t="s">
         <v>261</v>
-      </c>
-      <c r="H185" s="54" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="186" spans="1:8">
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="81"/>
+      <c r="B186" s="84"/>
       <c r="C186" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="D186" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E186" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F186" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="D186" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E186" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F186" s="51" t="s">
+      <c r="G186" s="70" t="s">
         <v>258</v>
       </c>
-      <c r="G186" s="70" t="s">
+      <c r="H186" s="54" t="s">
         <v>259</v>
-      </c>
-      <c r="H186" s="54" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="81"/>
+      <c r="B187" s="84"/>
       <c r="C187" s="51" t="s">
         <v>117</v>
       </c>
@@ -7481,7 +7423,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="81"/>
+      <c r="B188" s="84"/>
       <c r="C188" s="21" t="s">
         <v>118</v>
       </c>
@@ -7498,14 +7440,14 @@
         <v>20.03</v>
       </c>
       <c r="H188" s="54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="81"/>
+      <c r="B189" s="84"/>
       <c r="C189" s="21" t="s">
         <v>119</v>
       </c>
@@ -7527,7 +7469,7 @@
       <c r="A190" s="19">
         <v>42</v>
       </c>
-      <c r="B190" s="81"/>
+      <c r="B190" s="84"/>
       <c r="C190" s="21" t="s">
         <v>120</v>
       </c>
@@ -7547,7 +7489,7 @@
       <c r="A191" s="19">
         <v>43</v>
       </c>
-      <c r="B191" s="81"/>
+      <c r="B191" s="84"/>
       <c r="C191" s="21" t="s">
         <v>121</v>
       </c>
@@ -7567,7 +7509,7 @@
       <c r="A192" s="19">
         <v>44</v>
       </c>
-      <c r="B192" s="81"/>
+      <c r="B192" s="84"/>
       <c r="C192" s="21" t="s">
         <v>39</v>
       </c>
@@ -7587,7 +7529,7 @@
       <c r="A193" s="19">
         <v>45</v>
       </c>
-      <c r="B193" s="81"/>
+      <c r="B193" s="84"/>
       <c r="C193" s="21" t="s">
         <v>113</v>
       </c>
@@ -7598,20 +7540,20 @@
         <v>78</v>
       </c>
       <c r="F193" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G193" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="H193" s="71" t="s">
         <v>322</v>
-      </c>
-      <c r="H193" s="71" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="45">
       <c r="A194" s="19">
         <v>46</v>
       </c>
-      <c r="B194" s="80" t="s">
+      <c r="B194" s="85" t="s">
         <v>7</v>
       </c>
       <c r="C194" s="21" t="s">
@@ -7624,10 +7566,10 @@
         <v>78</v>
       </c>
       <c r="F194" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G194" s="58" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H194" s="11"/>
     </row>
@@ -7635,7 +7577,7 @@
       <c r="A195" s="19">
         <v>47</v>
       </c>
-      <c r="B195" s="81"/>
+      <c r="B195" s="84"/>
       <c r="C195" s="51" t="s">
         <v>123</v>
       </c>
@@ -7657,9 +7599,9 @@
       <c r="A196" s="19">
         <v>48</v>
       </c>
-      <c r="B196" s="81"/>
+      <c r="B196" s="84"/>
       <c r="C196" s="51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D196" s="21" t="s">
         <v>78</v>
@@ -7671,7 +7613,7 @@
         <v>124</v>
       </c>
       <c r="G196" s="51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H196" s="11"/>
     </row>
@@ -7679,7 +7621,7 @@
       <c r="A197" s="19">
         <v>49</v>
       </c>
-      <c r="B197" s="81"/>
+      <c r="B197" s="84"/>
       <c r="C197" s="51" t="s">
         <v>126</v>
       </c>
@@ -7690,10 +7632,10 @@
         <v>78</v>
       </c>
       <c r="F197" s="51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G197" s="51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H197" s="11"/>
     </row>
@@ -7701,9 +7643,9 @@
       <c r="A198" s="19">
         <v>50</v>
       </c>
-      <c r="B198" s="81"/>
+      <c r="B198" s="84"/>
       <c r="C198" s="51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D198" s="21" t="s">
         <v>78</v>
@@ -7715,7 +7657,7 @@
         <v>64</v>
       </c>
       <c r="G198" s="51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H198" s="11"/>
     </row>
@@ -7723,9 +7665,9 @@
       <c r="A199" s="19">
         <v>51</v>
       </c>
-      <c r="B199" s="81"/>
+      <c r="B199" s="84"/>
       <c r="C199" s="51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D199" s="21" t="s">
         <v>78</v>
@@ -7737,7 +7679,7 @@
         <v>7.9</v>
       </c>
       <c r="G199" s="51" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H199" s="11"/>
     </row>
@@ -7745,9 +7687,9 @@
       <c r="A200" s="19">
         <v>52</v>
       </c>
-      <c r="B200" s="81"/>
+      <c r="B200" s="84"/>
       <c r="C200" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D200" s="21" t="s">
         <v>78</v>
@@ -7757,19 +7699,19 @@
         <v>50</v>
       </c>
       <c r="G200" s="51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H200" s="54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="201" spans="1:8">
       <c r="A201" s="19">
         <v>53</v>
       </c>
-      <c r="B201" s="81"/>
+      <c r="B201" s="84"/>
       <c r="C201" s="51" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D201" s="21" t="s">
         <v>78</v>
@@ -7779,19 +7721,19 @@
         <v>50</v>
       </c>
       <c r="G201" s="51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H201" s="54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="202" spans="1:8">
       <c r="A202" s="19">
         <v>54</v>
       </c>
-      <c r="B202" s="81"/>
+      <c r="B202" s="84"/>
       <c r="C202" s="51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D202" s="21" t="s">
         <v>78</v>
@@ -7801,17 +7743,17 @@
         <v>10</v>
       </c>
       <c r="G202" s="51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H202" s="54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="203" spans="1:8">
       <c r="A203" s="19">
         <v>55</v>
       </c>
-      <c r="B203" s="81"/>
+      <c r="B203" s="84"/>
       <c r="C203" s="51" t="s">
         <v>113</v>
       </c>
@@ -7822,20 +7764,20 @@
         <v>78</v>
       </c>
       <c r="F203" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G203" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="H203" s="54" t="s">
         <v>322</v>
-      </c>
-      <c r="H203" s="54" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="204" spans="1:8">
       <c r="A204" s="19">
         <v>56</v>
       </c>
-      <c r="B204" s="88" t="s">
+      <c r="B204" s="94" t="s">
         <v>8</v>
       </c>
       <c r="C204" s="21" t="s">
@@ -7861,7 +7803,7 @@
       <c r="A205" s="19">
         <v>57</v>
       </c>
-      <c r="B205" s="85"/>
+      <c r="B205" s="95"/>
       <c r="C205" s="20" t="s">
         <v>130</v>
       </c>
@@ -7885,18 +7827,18 @@
       <c r="A206" s="19">
         <v>58</v>
       </c>
-      <c r="B206" s="85"/>
+      <c r="B206" s="95"/>
       <c r="C206" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D206" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E206" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F206" s="20" t="s">
         <v>238</v>
-      </c>
-      <c r="D206" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E206" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F206" s="20" t="s">
-        <v>239</v>
       </c>
       <c r="G206" s="20" t="s">
         <v>80</v>
@@ -7909,7 +7851,7 @@
       <c r="A207" s="19">
         <v>59</v>
       </c>
-      <c r="B207" s="86"/>
+      <c r="B207" s="96"/>
       <c r="C207" s="53" t="s">
         <v>113</v>
       </c>
@@ -7920,20 +7862,20 @@
         <v>78</v>
       </c>
       <c r="F207" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G207" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H207" s="22" t="s">
         <v>322</v>
-      </c>
-      <c r="H207" s="22" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:8">
       <c r="A208" s="16">
         <v>60</v>
       </c>
-      <c r="B208" s="89" t="s">
+      <c r="B208" s="97" t="s">
         <v>65</v>
       </c>
       <c r="C208" s="52" t="s">
@@ -7957,9 +7899,9 @@
       <c r="A209" s="63">
         <v>61</v>
       </c>
-      <c r="B209" s="90"/>
+      <c r="B209" s="98"/>
       <c r="C209" s="64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D209" s="62" t="s">
         <v>78</v>
@@ -7969,17 +7911,17 @@
         <v>140</v>
       </c>
       <c r="G209" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="H209" s="36" t="s">
         <v>301</v>
-      </c>
-      <c r="H209" s="36" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="210" spans="1:8">
       <c r="A210" s="63">
         <v>62</v>
       </c>
-      <c r="B210" s="91"/>
+      <c r="B210" s="99"/>
       <c r="C210" s="51" t="s">
         <v>135</v>
       </c>
@@ -8001,7 +7943,7 @@
       <c r="A211" s="63">
         <v>63</v>
       </c>
-      <c r="B211" s="92"/>
+      <c r="B211" s="100"/>
       <c r="C211" s="53" t="s">
         <v>138</v>
       </c>
@@ -8023,7 +7965,7 @@
       <c r="A212" s="63">
         <v>64</v>
       </c>
-      <c r="B212" s="92"/>
+      <c r="B212" s="100"/>
       <c r="C212" s="53" t="s">
         <v>139</v>
       </c>
@@ -8045,7 +7987,7 @@
       <c r="A213" s="63">
         <v>65</v>
       </c>
-      <c r="B213" s="92"/>
+      <c r="B213" s="100"/>
       <c r="C213" s="53" t="s">
         <v>142</v>
       </c>
@@ -8065,7 +8007,7 @@
       <c r="A214" s="63">
         <v>66</v>
       </c>
-      <c r="B214" s="92"/>
+      <c r="B214" s="100"/>
       <c r="C214" s="53" t="s">
         <v>217</v>
       </c>
@@ -8087,7 +8029,7 @@
       <c r="A215" s="63">
         <v>67</v>
       </c>
-      <c r="B215" s="92"/>
+      <c r="B215" s="100"/>
       <c r="C215" s="53" t="s">
         <v>221</v>
       </c>
@@ -8109,9 +8051,9 @@
       <c r="A216" s="63">
         <v>68</v>
       </c>
-      <c r="B216" s="92"/>
+      <c r="B216" s="100"/>
       <c r="C216" s="53" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D216" s="20" t="s">
         <v>78</v>
@@ -8142,13 +8084,13 @@
         <v>78</v>
       </c>
       <c r="F217" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G217" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="H217" s="25" t="s">
         <v>322</v>
-      </c>
-      <c r="H217" s="25" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -8166,22 +8108,22 @@
     </row>
     <row r="220" spans="1:8">
       <c r="B220" s="59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="221" spans="1:8">
       <c r="B221" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="222" spans="1:8">
       <c r="B222" s="72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" spans="1:8">
       <c r="B223" s="59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="15.75" thickBot="1">
@@ -8189,7 +8131,7 @@
         <v>146</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="15.75" thickBot="1">
@@ -8199,11 +8141,11 @@
       <c r="B234" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C234" s="94" t="s">
+      <c r="C234" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="D234" s="94"/>
-      <c r="E234" s="94"/>
+      <c r="D234" s="101"/>
+      <c r="E234" s="101"/>
       <c r="F234" s="32" t="s">
         <v>150</v>
       </c>
@@ -8212,17 +8154,17 @@
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="95" t="s">
+      <c r="A235" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="B235" s="87" t="s">
+      <c r="B235" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="C235" s="98" t="s">
+      <c r="C235" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="D235" s="99"/>
-      <c r="E235" s="99"/>
+      <c r="D235" s="105"/>
+      <c r="E235" s="105"/>
       <c r="F235" s="62" t="s">
         <v>155</v>
       </c>
@@ -8231,13 +8173,13 @@
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="96"/>
-      <c r="B236" s="97"/>
-      <c r="C236" s="100" t="s">
+      <c r="A236" s="82"/>
+      <c r="B236" s="103"/>
+      <c r="C236" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="D236" s="101"/>
-      <c r="E236" s="101"/>
+      <c r="D236" s="107"/>
+      <c r="E236" s="107"/>
       <c r="F236" s="20" t="s">
         <v>157</v>
       </c>
@@ -8246,15 +8188,15 @@
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="96"/>
-      <c r="B237" s="81" t="s">
+      <c r="A237" s="82"/>
+      <c r="B237" s="84" t="s">
         <v>158</v>
       </c>
-      <c r="C237" s="102" t="s">
+      <c r="C237" s="108" t="s">
         <v>159</v>
       </c>
-      <c r="D237" s="102"/>
-      <c r="E237" s="102"/>
+      <c r="D237" s="108"/>
+      <c r="E237" s="108"/>
       <c r="F237" s="21" t="s">
         <v>155</v>
       </c>
@@ -8263,13 +8205,13 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="96"/>
-      <c r="B238" s="81"/>
-      <c r="C238" s="100" t="s">
+      <c r="A238" s="82"/>
+      <c r="B238" s="84"/>
+      <c r="C238" s="106" t="s">
         <v>159</v>
       </c>
-      <c r="D238" s="100"/>
-      <c r="E238" s="100"/>
+      <c r="D238" s="106"/>
+      <c r="E238" s="106"/>
       <c r="F238" s="21" t="s">
         <v>157</v>
       </c>
@@ -8278,15 +8220,15 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="96"/>
-      <c r="B239" s="97" t="s">
+      <c r="A239" s="82"/>
+      <c r="B239" s="103" t="s">
         <v>160</v>
       </c>
-      <c r="C239" s="103" t="s">
+      <c r="C239" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="D239" s="104"/>
-      <c r="E239" s="105"/>
+      <c r="D239" s="110"/>
+      <c r="E239" s="111"/>
       <c r="F239" s="21" t="s">
         <v>155</v>
       </c>
@@ -8295,13 +8237,13 @@
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="96"/>
-      <c r="B240" s="87"/>
-      <c r="C240" s="103" t="s">
+      <c r="A240" s="82"/>
+      <c r="B240" s="89"/>
+      <c r="C240" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="D240" s="104"/>
-      <c r="E240" s="105"/>
+      <c r="D240" s="110"/>
+      <c r="E240" s="111"/>
       <c r="F240" s="21" t="s">
         <v>157</v>
       </c>
@@ -8310,15 +8252,15 @@
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="96"/>
-      <c r="B241" s="81" t="s">
+      <c r="A241" s="82"/>
+      <c r="B241" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="C241" s="102" t="s">
+      <c r="C241" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="D241" s="102"/>
-      <c r="E241" s="102"/>
+      <c r="D241" s="108"/>
+      <c r="E241" s="108"/>
       <c r="F241" s="21" t="s">
         <v>155</v>
       </c>
@@ -8327,13 +8269,13 @@
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="96"/>
-      <c r="B242" s="81"/>
-      <c r="C242" s="102" t="s">
+      <c r="A242" s="82"/>
+      <c r="B242" s="84"/>
+      <c r="C242" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="D242" s="102"/>
-      <c r="E242" s="102"/>
+      <c r="D242" s="108"/>
+      <c r="E242" s="108"/>
       <c r="F242" s="21" t="s">
         <v>157</v>
       </c>
@@ -8342,17 +8284,17 @@
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="96" t="s">
+      <c r="A243" s="82" t="s">
         <v>163</v>
       </c>
-      <c r="B243" s="81" t="s">
+      <c r="B243" s="84" t="s">
         <v>164</v>
       </c>
-      <c r="C243" s="80" t="s">
+      <c r="C243" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="D243" s="81"/>
-      <c r="E243" s="81"/>
+      <c r="D243" s="84"/>
+      <c r="E243" s="84"/>
       <c r="F243" s="21" t="s">
         <v>155</v>
       </c>
@@ -8361,13 +8303,13 @@
       </c>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="96"/>
-      <c r="B244" s="81"/>
-      <c r="C244" s="81" t="s">
+      <c r="A244" s="82"/>
+      <c r="B244" s="84"/>
+      <c r="C244" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="D244" s="81"/>
-      <c r="E244" s="81"/>
+      <c r="D244" s="84"/>
+      <c r="E244" s="84"/>
       <c r="F244" s="21" t="s">
         <v>157</v>
       </c>
@@ -8376,15 +8318,15 @@
       </c>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="96"/>
-      <c r="B245" s="81" t="s">
+      <c r="A245" s="82"/>
+      <c r="B245" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="C245" s="81" t="s">
+      <c r="C245" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="D245" s="81"/>
-      <c r="E245" s="81"/>
+      <c r="D245" s="84"/>
+      <c r="E245" s="84"/>
       <c r="F245" s="21" t="s">
         <v>155</v>
       </c>
@@ -8393,13 +8335,13 @@
       </c>
     </row>
     <row r="246" spans="1:7">
-      <c r="A246" s="96"/>
-      <c r="B246" s="81"/>
-      <c r="C246" s="81" t="s">
+      <c r="A246" s="82"/>
+      <c r="B246" s="84"/>
+      <c r="C246" s="84" t="s">
         <v>170</v>
       </c>
-      <c r="D246" s="81"/>
-      <c r="E246" s="81"/>
+      <c r="D246" s="84"/>
+      <c r="E246" s="84"/>
       <c r="F246" s="21" t="s">
         <v>157</v>
       </c>
@@ -8408,17 +8350,17 @@
       </c>
     </row>
     <row r="247" spans="1:7">
-      <c r="A247" s="96" t="s">
+      <c r="A247" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="B247" s="81" t="s">
+      <c r="B247" s="84" t="s">
         <v>172</v>
       </c>
-      <c r="C247" s="80" t="s">
+      <c r="C247" s="85" t="s">
         <v>173</v>
       </c>
-      <c r="D247" s="81"/>
-      <c r="E247" s="81"/>
+      <c r="D247" s="84"/>
+      <c r="E247" s="84"/>
       <c r="F247" s="21" t="s">
         <v>155</v>
       </c>
@@ -8427,13 +8369,13 @@
       </c>
     </row>
     <row r="248" spans="1:7">
-      <c r="A248" s="96"/>
-      <c r="B248" s="81"/>
-      <c r="C248" s="81" t="s">
+      <c r="A248" s="82"/>
+      <c r="B248" s="84"/>
+      <c r="C248" s="84" t="s">
         <v>174</v>
       </c>
-      <c r="D248" s="81"/>
-      <c r="E248" s="81"/>
+      <c r="D248" s="84"/>
+      <c r="E248" s="84"/>
       <c r="F248" s="21" t="s">
         <v>157</v>
       </c>
@@ -8442,15 +8384,15 @@
       </c>
     </row>
     <row r="249" spans="1:7">
-      <c r="A249" s="96"/>
-      <c r="B249" s="81" t="s">
+      <c r="A249" s="82"/>
+      <c r="B249" s="84" t="s">
         <v>175</v>
       </c>
-      <c r="C249" s="80" t="s">
+      <c r="C249" s="85" t="s">
         <v>176</v>
       </c>
-      <c r="D249" s="81"/>
-      <c r="E249" s="81"/>
+      <c r="D249" s="84"/>
+      <c r="E249" s="84"/>
       <c r="F249" s="21" t="s">
         <v>155</v>
       </c>
@@ -8459,13 +8401,13 @@
       </c>
     </row>
     <row r="250" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A250" s="107"/>
-      <c r="B250" s="108"/>
-      <c r="C250" s="108" t="s">
+      <c r="A250" s="83"/>
+      <c r="B250" s="86"/>
+      <c r="C250" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="D250" s="108"/>
-      <c r="E250" s="108"/>
+      <c r="D250" s="86"/>
+      <c r="E250" s="86"/>
       <c r="F250" s="24" t="s">
         <v>157</v>
       </c>
@@ -8487,12 +8429,12 @@
       <c r="A255" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="B255" s="109" t="s">
+      <c r="B255" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="C255" s="109"/>
-      <c r="D255" s="109"/>
-      <c r="E255" s="109"/>
+      <c r="C255" s="87"/>
+      <c r="D255" s="87"/>
+      <c r="E255" s="87"/>
       <c r="F255" s="32" t="s">
         <v>182</v>
       </c>
@@ -8504,12 +8446,12 @@
       <c r="A256" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="B256" s="110" t="s">
+      <c r="B256" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="C256" s="87"/>
-      <c r="D256" s="87"/>
-      <c r="E256" s="87"/>
+      <c r="C256" s="89"/>
+      <c r="D256" s="89"/>
+      <c r="E256" s="89"/>
       <c r="F256" s="35" t="s">
         <v>63</v>
       </c>
@@ -8521,12 +8463,12 @@
       <c r="A257" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B257" s="111" t="s">
+      <c r="B257" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="C257" s="112"/>
-      <c r="D257" s="112"/>
-      <c r="E257" s="113"/>
+      <c r="C257" s="91"/>
+      <c r="D257" s="91"/>
+      <c r="E257" s="92"/>
       <c r="F257" s="9" t="s">
         <v>156</v>
       </c>
@@ -8538,12 +8480,12 @@
       <c r="A258" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B258" s="111" t="s">
+      <c r="B258" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="C258" s="112"/>
-      <c r="D258" s="112"/>
-      <c r="E258" s="113"/>
+      <c r="C258" s="91"/>
+      <c r="D258" s="91"/>
+      <c r="E258" s="92"/>
       <c r="F258" s="13" t="s">
         <v>156</v>
       </c>
@@ -8558,9 +8500,9 @@
       <c r="B259" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="C259" s="108"/>
-      <c r="D259" s="108"/>
-      <c r="E259" s="108"/>
+      <c r="C259" s="86"/>
+      <c r="D259" s="86"/>
+      <c r="E259" s="86"/>
       <c r="F259" s="15" t="s">
         <v>156</v>
       </c>
@@ -8605,11 +8547,11 @@
       <c r="C264" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="D264" s="106" t="s">
+      <c r="D264" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="E264" s="106"/>
-      <c r="F264" s="106"/>
+      <c r="E264" s="81"/>
+      <c r="F264" s="81"/>
       <c r="G264" s="18"/>
     </row>
     <row r="265" spans="1:7">
@@ -8622,11 +8564,11 @@
       <c r="C265" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D265" s="114" t="s">
+      <c r="D265" s="80" t="s">
         <v>198</v>
       </c>
-      <c r="E265" s="114"/>
-      <c r="F265" s="114"/>
+      <c r="E265" s="80"/>
+      <c r="F265" s="80"/>
       <c r="G265" s="28"/>
     </row>
     <row r="266" spans="1:7">
@@ -8639,11 +8581,11 @@
       <c r="C266" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D266" s="114" t="s">
+      <c r="D266" s="80" t="s">
         <v>199</v>
       </c>
-      <c r="E266" s="114"/>
-      <c r="F266" s="114"/>
+      <c r="E266" s="80"/>
+      <c r="F266" s="80"/>
       <c r="G266" s="28"/>
     </row>
     <row r="267" spans="1:7">
@@ -8656,11 +8598,11 @@
       <c r="C267" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D267" s="114" t="s">
+      <c r="D267" s="80" t="s">
         <v>200</v>
       </c>
-      <c r="E267" s="114"/>
-      <c r="F267" s="114"/>
+      <c r="E267" s="80"/>
+      <c r="F267" s="80"/>
       <c r="G267" s="28"/>
     </row>
     <row r="268" spans="1:7">
@@ -8673,11 +8615,11 @@
       <c r="C268" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D268" s="114" t="s">
+      <c r="D268" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="E268" s="114"/>
-      <c r="F268" s="114"/>
+      <c r="E268" s="80"/>
+      <c r="F268" s="80"/>
       <c r="G268" s="28"/>
     </row>
     <row r="269" spans="1:7">
@@ -8690,11 +8632,11 @@
       <c r="C269" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D269" s="114" t="s">
+      <c r="D269" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="E269" s="114"/>
-      <c r="F269" s="114"/>
+      <c r="E269" s="80"/>
+      <c r="F269" s="80"/>
       <c r="G269" s="28"/>
     </row>
     <row r="270" spans="1:7">
@@ -8707,11 +8649,11 @@
       <c r="C270" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D270" s="114" t="s">
+      <c r="D270" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="E270" s="114"/>
-      <c r="F270" s="114"/>
+      <c r="E270" s="80"/>
+      <c r="F270" s="80"/>
       <c r="G270" s="28"/>
     </row>
     <row r="271" spans="1:7">
@@ -8724,11 +8666,11 @@
       <c r="C271" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D271" s="114" t="s">
+      <c r="D271" s="80" t="s">
         <v>204</v>
       </c>
-      <c r="E271" s="114"/>
-      <c r="F271" s="114"/>
+      <c r="E271" s="80"/>
+      <c r="F271" s="80"/>
       <c r="G271" s="28"/>
     </row>
     <row r="272" spans="1:7">
@@ -8741,11 +8683,11 @@
       <c r="C272" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D272" s="114" t="s">
+      <c r="D272" s="80" t="s">
         <v>205</v>
       </c>
-      <c r="E272" s="114"/>
-      <c r="F272" s="114"/>
+      <c r="E272" s="80"/>
+      <c r="F272" s="80"/>
       <c r="G272" s="28"/>
     </row>
     <row r="273" spans="1:7">
@@ -8861,7 +8803,7 @@
         <v>196</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E279" s="9"/>
       <c r="F279" s="9"/>
@@ -8878,7 +8820,7 @@
         <v>196</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E280" s="9"/>
       <c r="F280" s="9"/>
@@ -8895,7 +8837,7 @@
         <v>196</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E281" s="9"/>
       <c r="F281" s="9"/>
@@ -8912,7 +8854,7 @@
         <v>196</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E282" s="9"/>
       <c r="F282" s="9"/>
@@ -8929,7 +8871,7 @@
         <v>196</v>
       </c>
       <c r="D283" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E283" s="9"/>
       <c r="F283" s="9"/>
@@ -8946,7 +8888,7 @@
         <v>196</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E284" s="9"/>
       <c r="F284" s="9"/>
@@ -8963,7 +8905,7 @@
         <v>196</v>
       </c>
       <c r="D285" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E285" s="9"/>
       <c r="F285" s="9"/>
@@ -8980,7 +8922,7 @@
         <v>196</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E286" s="9"/>
       <c r="F286" s="9"/>
@@ -8997,7 +8939,7 @@
         <v>196</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E287" s="9"/>
       <c r="F287" s="9"/>
@@ -9014,7 +8956,7 @@
         <v>196</v>
       </c>
       <c r="D288" s="57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E288" s="9"/>
       <c r="F288" s="9"/>
@@ -9031,7 +8973,7 @@
         <v>196</v>
       </c>
       <c r="D289" s="75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E289" s="13"/>
       <c r="F289" s="13"/>
@@ -9048,7 +8990,7 @@
         <v>196</v>
       </c>
       <c r="D290" s="69" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E290" s="15"/>
       <c r="F290" s="15"/>
@@ -9057,34 +8999,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="2ZwYjp9JQKNmLpcvubwUpkakqpvbxMGUDX2YfB8P44tj3Eex5wtoKK5M/5zR2d0nfJdohweGomUTjqHGzUDKNg==" saltValue="oPopBuSQ5MZ4FNcEjcsJ1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="50">
-    <mergeCell ref="D271:F271"/>
-    <mergeCell ref="D272:F272"/>
-    <mergeCell ref="D265:F265"/>
-    <mergeCell ref="D266:F266"/>
-    <mergeCell ref="D267:F267"/>
-    <mergeCell ref="D268:F268"/>
-    <mergeCell ref="D269:F269"/>
-    <mergeCell ref="D270:F270"/>
-    <mergeCell ref="D264:F264"/>
-    <mergeCell ref="A247:A250"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="C247:E247"/>
-    <mergeCell ref="C248:E248"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="C249:E249"/>
-    <mergeCell ref="C250:E250"/>
-    <mergeCell ref="B255:E255"/>
-    <mergeCell ref="B256:E256"/>
-    <mergeCell ref="B257:E257"/>
-    <mergeCell ref="B258:E258"/>
-    <mergeCell ref="B259:E259"/>
-    <mergeCell ref="A243:A246"/>
-    <mergeCell ref="B243:B244"/>
-    <mergeCell ref="C243:E243"/>
-    <mergeCell ref="C244:E244"/>
-    <mergeCell ref="B245:B246"/>
-    <mergeCell ref="C245:E245"/>
-    <mergeCell ref="C246:E246"/>
+    <mergeCell ref="B194:B203"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B149:B164"/>
+    <mergeCell ref="B165:B173"/>
+    <mergeCell ref="B174:B184"/>
+    <mergeCell ref="B185:B193"/>
     <mergeCell ref="B204:B207"/>
     <mergeCell ref="B208:B217"/>
     <mergeCell ref="C234:E234"/>
@@ -9101,12 +9021,34 @@
     <mergeCell ref="B241:B242"/>
     <mergeCell ref="C241:E241"/>
     <mergeCell ref="C242:E242"/>
-    <mergeCell ref="B194:B203"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B149:B164"/>
-    <mergeCell ref="B165:B173"/>
-    <mergeCell ref="B174:B184"/>
-    <mergeCell ref="B185:B193"/>
+    <mergeCell ref="A243:A246"/>
+    <mergeCell ref="B243:B244"/>
+    <mergeCell ref="C243:E243"/>
+    <mergeCell ref="C244:E244"/>
+    <mergeCell ref="B245:B246"/>
+    <mergeCell ref="C245:E245"/>
+    <mergeCell ref="C246:E246"/>
+    <mergeCell ref="D264:F264"/>
+    <mergeCell ref="A247:A250"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="C247:E247"/>
+    <mergeCell ref="C248:E248"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="C249:E249"/>
+    <mergeCell ref="C250:E250"/>
+    <mergeCell ref="B255:E255"/>
+    <mergeCell ref="B256:E256"/>
+    <mergeCell ref="B257:E257"/>
+    <mergeCell ref="B258:E258"/>
+    <mergeCell ref="B259:E259"/>
+    <mergeCell ref="D271:F271"/>
+    <mergeCell ref="D272:F272"/>
+    <mergeCell ref="D265:F265"/>
+    <mergeCell ref="D266:F266"/>
+    <mergeCell ref="D267:F267"/>
+    <mergeCell ref="D268:F268"/>
+    <mergeCell ref="D269:F269"/>
+    <mergeCell ref="D270:F270"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9132,16 +9074,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>